<commit_message>
updated scripts - doc upload support
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mibin.boban/Documents/Solutions/ccs-enterprise-automation-ui-project/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B3DACD-57AC-274E-A45B-8B3054151C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755352A1-3361-3942-A918-9B308CDB4BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1760" yWindow="2020" windowWidth="26200" windowHeight="12940" tabRatio="752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="11" r:id="rId1"/>
     <sheet name="TestCases" sheetId="4" r:id="rId2"/>
-    <sheet name="TC001_VisualTesting" sheetId="12" r:id="rId3"/>
-    <sheet name="TC001_SignIn" sheetId="3" r:id="rId4"/>
-    <sheet name="TC002_Login" sheetId="10" r:id="rId5"/>
+    <sheet name="TC002_FileUpload" sheetId="13" r:id="rId3"/>
+    <sheet name="TC001_VisualTesting" sheetId="12" r:id="rId4"/>
+    <sheet name="TC001_SignIn" sheetId="3" r:id="rId5"/>
+    <sheet name="TC002_Login" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="179">
   <si>
     <t>TS_02</t>
   </si>
@@ -665,6 +666,33 @@
   </si>
   <si>
     <t>To uncheck a checkbox if already selected</t>
+  </si>
+  <si>
+    <t>UploadFile</t>
+  </si>
+  <si>
+    <t>TC002_FileUpload</t>
+  </si>
+  <si>
+    <t>To upload a file</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>elm_upload</t>
+  </si>
+  <si>
+    <t>Upload a file</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>/src/test/resources/inputFiles/testFileupload.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To upload a file. Add files under src/test/resources/inputFiles. Provide value as path from content root (right click on file &gt; copy path or reference &gt; copy path from content root. Add '/' at the beginning (Eg: /src/test/resources/inputFiles/testFileupload.txt) </t>
   </si>
 </sst>
 </file>
@@ -1184,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1D0990-AD1B-5244-AC3C-8B60408730A0}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1516,6 +1544,14 @@
         <v>169</v>
       </c>
     </row>
+    <row r="41" spans="1:2" ht="40" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1524,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1561,9 +1597,23 @@
         <v>96</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1576,11 +1626,82 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218E4CAA-8CE3-9A43-98B7-0937BA1D7CB8}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="45.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2F9272-E435-A340-8F70-AC025BC35780}">
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2045,12 +2166,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2181,7 +2302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E711B2E9-84E6-C647-AF41-931D98C86C3E}">
   <dimension ref="A1:E6"/>
   <sheetViews>

</xml_diff>